<commit_message>
Midterm data and minor updates from class.
</commit_message>
<xml_diff>
--- a/testfiles/Tests.xlsx
+++ b/testfiles/Tests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dumacduke-my.sharepoint.com/personal/dpazzula_dumac_duke_edu/Documents/Documents/FinTech-545-Fall2025/testfiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="79" documentId="13_ncr:1_{13B31C93-206E-4E64-980E-4155A2D902A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DD445982-174F-435E-93B5-6550AA4DEB50}"/>
+  <xr:revisionPtr revIDLastSave="97" documentId="13_ncr:1_{13B31C93-206E-4E64-980E-4155A2D902A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2DD18703-B64B-44CA-A4C9-1F850B5B7B30}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-36690" yWindow="-2895" windowWidth="23670" windowHeight="17940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -561,18 +561,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="61.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.54296875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.1796875" customWidth="1"/>
+    <col min="4" max="4" width="15.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -586,7 +586,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1.1000000000000001</v>
       </c>
@@ -601,7 +601,7 @@
         <v>testout_1.1.csv</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1.2</v>
       </c>
@@ -616,7 +616,7 @@
         <v>testout_1.2.csv</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1.3</v>
       </c>
@@ -631,7 +631,7 @@
         <v>testout_1.3.csv</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1.4</v>
       </c>
@@ -646,7 +646,7 @@
         <v>testout_1.4.csv</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2.1</v>
       </c>
@@ -661,7 +661,7 @@
         <v>testout_2.1.csv</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2.2000000000000002</v>
       </c>
@@ -676,7 +676,7 @@
         <v>testout_2.2.csv</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>2.2999999999999998</v>
       </c>
@@ -691,7 +691,7 @@
         <v>testout_2.3.csv</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>3.1</v>
       </c>
@@ -706,7 +706,7 @@
         <v>testout_3.1.csv</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>3.2</v>
       </c>
@@ -721,7 +721,7 @@
         <v>testout_3.2.csv</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>3.3</v>
       </c>
@@ -736,7 +736,7 @@
         <v>testout_3.3.csv</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>3.4</v>
       </c>
@@ -751,7 +751,7 @@
         <v>testout_3.4.csv</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>4.0999999999999996</v>
       </c>
@@ -766,7 +766,7 @@
         <v>testout_4.1.csv</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>5.0999999999999996</v>
       </c>
@@ -781,7 +781,7 @@
         <v>testout_5.1.csv</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>5.2</v>
       </c>
@@ -796,7 +796,7 @@
         <v>testout_5.2.csv</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>5.3</v>
       </c>
@@ -811,7 +811,7 @@
         <v>testout_5.3.csv</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>5.4</v>
       </c>
@@ -826,7 +826,7 @@
         <v>testout_5.4.csv</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>5.5</v>
       </c>
@@ -841,7 +841,7 @@
         <v>testout_5.5.csv</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>6.1</v>
       </c>
@@ -856,7 +856,7 @@
         <v>testout_6.1.csv</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>6.2</v>
       </c>
@@ -871,7 +871,7 @@
         <v>testout_6.2.csv</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>7.1</v>
       </c>
@@ -886,7 +886,7 @@
         <v>testout_7.1.csv</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>7.2</v>
       </c>
@@ -901,7 +901,7 @@
         <v>testout_7.2.csv</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>7.3</v>
       </c>
@@ -916,7 +916,7 @@
         <v>testout_7.3.csv</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>7.4</v>
       </c>
@@ -931,7 +931,7 @@
         <v>testout_7.4.csv</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>8.1</v>
       </c>
@@ -946,7 +946,7 @@
         <v>testout_8.1.csv</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>8.1999999999999993</v>
       </c>
@@ -961,7 +961,7 @@
         <v>testout_8.2.csv</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>8.3000000000000007</v>
       </c>
@@ -976,7 +976,7 @@
         <v>testout_8.3.csv</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>8.4</v>
       </c>
@@ -991,7 +991,7 @@
         <v>testout_8.4.csv</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>8.5</v>
       </c>
@@ -1006,7 +1006,7 @@
         <v>testout_8.5.csv</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>8.6</v>
       </c>
@@ -1021,7 +1021,7 @@
         <v>testout_8.6.csv</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>9.1</v>
       </c>
@@ -1036,7 +1036,7 @@
         <v>testout_9.1.csv</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>10.1</v>
       </c>
@@ -1051,7 +1051,7 @@
         <v>testout_10.1.csv</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>10.199999999999999</v>
       </c>
@@ -1066,7 +1066,7 @@
         <v>testout_10.2.csv</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>10.3</v>
       </c>
@@ -1081,7 +1081,7 @@
         <v>testout_10.3.csv</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>10.4</v>
       </c>
@@ -1096,7 +1096,7 @@
         <v>testout_10.4.csv</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>11.1</v>
       </c>
@@ -1111,7 +1111,7 @@
         <v>testout_11.1.csv</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="87" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>11.2</v>
       </c>
@@ -1126,7 +1126,7 @@
         <v>testout_11.2.csv</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>12.1</v>
       </c>
@@ -1141,7 +1141,7 @@
         <v>testout_12.1.csv</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>12.2</v>
       </c>
@@ -1156,7 +1156,7 @@
         <v>testout_12.2.csv</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>12.3</v>
       </c>

</xml_diff>